<commit_message>
AP z boson CMS 8 TeV
</commit_message>
<xml_diff>
--- a/z_qT/expdata/10001.xlsx
+++ b/z_qT/expdata/10001.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avp5627/GIT/fitpack2/database/z_qT/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8E687C6A-AFF0-DD4A-8F81-82039029ED15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9E8B3A-DB11-DC40-9872-6D18BA32E995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="2480" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="3060" yWindow="2480" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CMS13-00y04-norm" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="30">
   <si>
     <t>FiducialCuts</t>
   </si>
@@ -116,11 +116,17 @@
   <si>
     <t>ktCut1[GeV]</t>
   </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>pp-&gt;Z/gamma*-&gt;l+ l-</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -963,16 +969,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AB35" sqref="AB35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1045,8 +1051,11 @@
       <c r="X1" t="s">
         <v>26</v>
       </c>
+      <c r="Y1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>SQRT(169000000)</f>
         <v>13000</v>
@@ -1121,8 +1130,11 @@
       <c r="X2" t="s">
         <v>25</v>
       </c>
+      <c r="Y2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>SQRT(169000000)</f>
         <v>13000</v>
@@ -1197,8 +1209,11 @@
       <c r="X3" t="s">
         <v>25</v>
       </c>
+      <c r="Y3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A35" si="1">SQRT(169000000)</f>
         <v>13000</v>
@@ -1273,8 +1288,11 @@
       <c r="X4" t="s">
         <v>25</v>
       </c>
+      <c r="Y4" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1349,8 +1367,11 @@
       <c r="X5" t="s">
         <v>25</v>
       </c>
+      <c r="Y5" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1425,8 +1446,11 @@
       <c r="X6" t="s">
         <v>25</v>
       </c>
+      <c r="Y6" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1501,8 +1525,11 @@
       <c r="X7" t="s">
         <v>25</v>
       </c>
+      <c r="Y7" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1577,8 +1604,11 @@
       <c r="X8" t="s">
         <v>25</v>
       </c>
+      <c r="Y8" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1653,8 +1683,11 @@
       <c r="X9" t="s">
         <v>25</v>
       </c>
+      <c r="Y9" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1729,8 +1762,11 @@
       <c r="X10" t="s">
         <v>25</v>
       </c>
+      <c r="Y10" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1805,8 +1841,11 @@
       <c r="X11" t="s">
         <v>25</v>
       </c>
+      <c r="Y11" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1881,8 +1920,11 @@
       <c r="X12" t="s">
         <v>25</v>
       </c>
+      <c r="Y12" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1957,8 +1999,11 @@
       <c r="X13" t="s">
         <v>25</v>
       </c>
+      <c r="Y13" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2033,8 +2078,11 @@
       <c r="X14" t="s">
         <v>25</v>
       </c>
+      <c r="Y14" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2109,8 +2157,11 @@
       <c r="X15" t="s">
         <v>25</v>
       </c>
+      <c r="Y15" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2185,8 +2236,11 @@
       <c r="X16" t="s">
         <v>25</v>
       </c>
+      <c r="Y16" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2261,8 +2315,11 @@
       <c r="X17" t="s">
         <v>25</v>
       </c>
+      <c r="Y17" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2337,8 +2394,11 @@
       <c r="X18" t="s">
         <v>25</v>
       </c>
+      <c r="Y18" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2413,8 +2473,11 @@
       <c r="X19" t="s">
         <v>25</v>
       </c>
+      <c r="Y19" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2489,8 +2552,11 @@
       <c r="X20" t="s">
         <v>25</v>
       </c>
+      <c r="Y20" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2565,8 +2631,11 @@
       <c r="X21" t="s">
         <v>25</v>
       </c>
+      <c r="Y21" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2641,8 +2710,11 @@
       <c r="X22" t="s">
         <v>25</v>
       </c>
+      <c r="Y22" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2717,8 +2789,11 @@
       <c r="X23" t="s">
         <v>25</v>
       </c>
+      <c r="Y23" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2793,8 +2868,11 @@
       <c r="X24" t="s">
         <v>25</v>
       </c>
+      <c r="Y24" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2869,8 +2947,11 @@
       <c r="X25" t="s">
         <v>25</v>
       </c>
+      <c r="Y25" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2945,8 +3026,11 @@
       <c r="X26" t="s">
         <v>25</v>
       </c>
+      <c r="Y26" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3021,8 +3105,11 @@
       <c r="X27" t="s">
         <v>25</v>
       </c>
+      <c r="Y27" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3097,8 +3184,11 @@
       <c r="X28" t="s">
         <v>25</v>
       </c>
+      <c r="Y28" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3173,8 +3263,11 @@
       <c r="X29" t="s">
         <v>25</v>
       </c>
+      <c r="Y29" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3249,8 +3342,11 @@
       <c r="X30" t="s">
         <v>25</v>
       </c>
+      <c r="Y30" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3325,8 +3421,11 @@
       <c r="X31" t="s">
         <v>25</v>
       </c>
+      <c r="Y31" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3401,8 +3500,11 @@
       <c r="X32" t="s">
         <v>25</v>
       </c>
+      <c r="Y32" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3477,8 +3579,11 @@
       <c r="X33" t="s">
         <v>25</v>
       </c>
+      <c r="Y33" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3553,8 +3658,11 @@
       <c r="X34" t="s">
         <v>25</v>
       </c>
+      <c r="Y34" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3628,6 +3736,9 @@
       </c>
       <c r="X35" t="s">
         <v>25</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>